<commit_message>
fixed s error now has problem with /n
</commit_message>
<xml_diff>
--- a/etc/Clue_map.xlsx
+++ b/etc/Clue_map.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="21075" windowHeight="10545"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="20730" windowHeight="10545"/>
   </bookViews>
   <sheets>
     <sheet name="Clue_map" sheetId="1" r:id="rId1"/>
@@ -949,8 +949,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="J27" sqref="J27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>